<commit_message>
Added first order reduction
</commit_message>
<xml_diff>
--- a/concepts/Goal Reduction.xlsx
+++ b/concepts/Goal Reduction.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Setup n Result" sheetId="1" r:id="rId1"/>
-    <sheet name="Statements" sheetId="2" r:id="rId2"/>
+    <sheet name="Statements Theoretical" sheetId="2" r:id="rId2"/>
+    <sheet name="Statements Empirical" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="228">
   <si>
     <t xml:space="preserve">[[e, inside, l], [l, ontop, g], [g, inside, l], [l, leftof, e], [e, inside, l]], </t>
   </si>
@@ -375,6 +376,330 @@
   </si>
   <si>
     <t>5 order reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, l] [leftof, l, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, l] [leftof, l, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, l] [leftof, l, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, l] [leftof, l, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, l] [leftof, l, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, l] [leftof, l, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, k] [leftof, k, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, k] [leftof, k, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, k] [leftof, k, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, k] [leftof, k, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, k] [leftof, k, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, k] [leftof, k, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, m] [leftof, m, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, m] [leftof, m, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, m] [leftof, m, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, m] [leftof, m, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, m] [leftof, m, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, l] [ontop, l, g] [inside, g, m] [leftof, m, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, l] [leftof, l, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, l] [leftof, l, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, l] [leftof, l, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, l] [leftof, l, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, l] [leftof, l, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, l] [leftof, l, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, k] [leftof, k, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, k] [leftof, k, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, k] [leftof, k, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, k] [leftof, k, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, k] [leftof, k, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, k] [leftof, k, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, m] [leftof, m, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, m] [leftof, m, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, m] [leftof, m, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, m] [leftof, m, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, m] [leftof, m, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, k] [ontop, k, g] [inside, g, m] [leftof, m, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, l] [leftof, l, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, l] [leftof, l, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, l] [leftof, l, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, l] [leftof, l, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, l] [leftof, l, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, l] [leftof, l, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, k] [leftof, k, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, k] [leftof, k, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, k] [leftof, k, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, k] [leftof, k, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, k] [leftof, k, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, k] [leftof, k, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, m] [leftof, m, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, m] [leftof, m, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, m] [leftof, m, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, m] [leftof, m, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, m] [leftof, m, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, e, m] [ontop, m, g] [inside, g, m] [leftof, m, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, l] [leftof, l, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, l] [leftof, l, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, l] [leftof, l, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, l] [leftof, l, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, l] [leftof, l, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, l] [leftof, l, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, k] [leftof, k, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, k] [leftof, k, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, k] [leftof, k, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, k] [leftof, k, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, k] [leftof, k, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, k] [leftof, k, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, m] [leftof, m, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, m] [leftof, m, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, m] [leftof, m, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, m] [leftof, m, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, m] [leftof, m, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, l] [ontop, l, g] [inside, g, m] [leftof, m, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, l] [leftof, l, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, l] [leftof, l, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, l] [leftof, l, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, l] [leftof, l, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, l] [leftof, l, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, l] [leftof, l, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, k] [leftof, k, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, k] [leftof, k, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, k] [leftof, k, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, k] [leftof, k, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, k] [leftof, k, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, k] [leftof, k, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, m] [leftof, m, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, m] [leftof, m, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, m] [leftof, m, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, m] [leftof, m, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, m] [leftof, m, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, k] [ontop, k, g] [inside, g, m] [leftof, m, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, l] [leftof, l, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, l] [leftof, l, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, l] [leftof, l, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, l] [leftof, l, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, l] [leftof, l, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, l] [leftof, l, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, k] [leftof, k, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, k] [leftof, k, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, k] [leftof, k, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, k] [leftof, k, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, k] [leftof, k, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, k] [leftof, k, f] [inside, f, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, m] [leftof, m, e] [inside, e, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, m] [leftof, m, e] [inside, e, k] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, m] [leftof, m, e] [inside, e, m] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, m] [leftof, m, f] [inside, f, l] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[inside, f, m] [ontop, m, g] [inside, g, m] [leftof, m, f] [inside, f, k] </t>
+  </si>
+  <si>
+    <t>[inside, f, m] [ontop, m, g] [inside, g, m] [leftof, m, f] [inside, f, m]</t>
   </si>
 </sst>
 </file>
@@ -709,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:D14"/>
+  <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -722,7 +1047,7 @@
     <col min="5" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>108</v>
       </c>
@@ -730,12 +1055,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:5">
       <c r="C4" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>110</v>
       </c>
@@ -743,67 +1068,95 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:5">
       <c r="C7" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D7">
-        <f>COUNTIF(Statements!A:A,"*")</f>
+        <f>COUNTIF('Statements Theoretical'!A:A,"*")</f>
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="E7">
+        <f>COUNTIF('Statements Empirical'!A:A,"*")</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
       <c r="C8" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D8">
-        <f>COUNTIF(Statements!B:B,"*")</f>
+        <f>COUNTIF('Statements Theoretical'!B:B,"*")</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
+      <c r="E8">
+        <f>COUNTIF('Statements Empirical'!B:B,"*")</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
       <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D9">
-        <f>COUNTIF(Statements!C:C,"*")</f>
+        <f>COUNTIF('Statements Theoretical'!C:C,"*")</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="E9">
+        <f>COUNTIF('Statements Empirical'!C:C,"*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
       <c r="C10" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D10">
-        <f>COUNTIF(Statements!D:D,"*")</f>
+        <f>COUNTIF('Statements Theoretical'!D:D,"*")</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:4">
+      <c r="E10">
+        <f>COUNTIF('Statements Empirical'!D:D,"*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
       <c r="C11" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D11">
-        <f>COUNTIF(Statements!E:E,"*")</f>
+        <f>COUNTIF('Statements Theoretical'!E:E,"*")</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="2:4">
+      <c r="E11">
+        <f>COUNTIF('Statements Empirical'!E:E,"*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
       <c r="C12" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D12">
-        <f>COUNTIF(Statements!F:F,"*")</f>
+        <f>COUNTIF('Statements Theoretical'!F:F,"*")</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:4">
+      <c r="E12">
+        <f>COUNTIF('Statements Empirical'!F:F,"*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
       <c r="C14" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D14">
-        <f>COUNTIF(Statements!H:H,"*")</f>
+        <f>COUNTIF('Statements Theoretical'!H:H,"*")</f>
         <v>4</v>
+      </c>
+      <c r="E14">
+        <f>COUNTIF('Statements Empirical'!H:H,"*")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1666,4 +2019,713 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B108"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>162</v>
+      </c>
+      <c r="B43" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added second order reduction, kind off
</commit_message>
<xml_diff>
--- a/concepts/Goal Reduction.xlsx
+++ b/concepts/Goal Reduction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup n Result" sheetId="1" r:id="rId1"/>
@@ -1036,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1153,10 +1153,6 @@
       <c r="D14">
         <f>COUNTIF('Statements Theoretical'!H:H,"*")</f>
         <v>4</v>
-      </c>
-      <c r="E14">
-        <f>COUNTIF('Statements Empirical'!H:H,"*")</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2025,14 +2021,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="62.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
added some notes on combined goals
</commit_message>
<xml_diff>
--- a/concepts/Goal Reduction.xlsx
+++ b/concepts/Goal Reduction.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Setup n Result" sheetId="1" r:id="rId1"/>
     <sheet name="Statements Theoretical" sheetId="2" r:id="rId2"/>
     <sheet name="Statements Empirical" sheetId="3" r:id="rId3"/>
+    <sheet name="Combined Goals Reduction" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="260">
   <si>
     <t xml:space="preserve">[[e, inside, l], [l, ontop, g], [g, inside, l], [l, leftof, e], [e, inside, l]], </t>
   </si>
@@ -706,6 +707,96 @@
   </si>
   <si>
     <t>Empirical</t>
+  </si>
+  <si>
+    <t>a in c, c on e</t>
+  </si>
+  <si>
+    <t>b in d, d on e</t>
+  </si>
+  <si>
+    <t>b in d, d on f</t>
+  </si>
+  <si>
+    <t>a in c, c on f</t>
+  </si>
+  <si>
+    <t>b in c, c on e</t>
+  </si>
+  <si>
+    <t>b in c, c on f</t>
+  </si>
+  <si>
+    <t>if relation = in || on</t>
+  </si>
+  <si>
+    <t>check taboo list</t>
+  </si>
+  <si>
+    <t>add obj1 to taboolist1</t>
+  </si>
+  <si>
+    <t>add obj2 to taboolist2</t>
+  </si>
+  <si>
+    <t>if first statement</t>
+  </si>
+  <si>
+    <t>add obj1 to taboolist2</t>
+  </si>
+  <si>
+    <t>if last statement</t>
+  </si>
+  <si>
+    <t>add obj2 to taboolist1</t>
+  </si>
+  <si>
+    <t>Check 1</t>
+  </si>
+  <si>
+    <t>a in c, c left of e</t>
+  </si>
+  <si>
+    <t>b in d, d left of e</t>
+  </si>
+  <si>
+    <t>b in d, d left of f</t>
+  </si>
+  <si>
+    <t>a in c, c left of f</t>
+  </si>
+  <si>
+    <t>b in c, c left of e</t>
+  </si>
+  <si>
+    <t>b in c, c left of f</t>
+  </si>
+  <si>
+    <t>Check 2</t>
+  </si>
+  <si>
+    <t>the reverse pair must never exist</t>
+  </si>
+  <si>
+    <t>such that</t>
+  </si>
+  <si>
+    <t>a left of c and c left of a does not occure</t>
+  </si>
+  <si>
+    <t>b right of d, d left of c</t>
+  </si>
+  <si>
+    <t>a right of c, c left of d</t>
+  </si>
+  <si>
+    <t>b right of c, c left of d</t>
+  </si>
+  <si>
+    <t>put a ball right of all boxes left of a box</t>
+  </si>
+  <si>
+    <t>a right of d, d left of c</t>
   </si>
 </sst>
 </file>
@@ -741,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -749,6 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,7 +1138,7 @@
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1186,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2802,4 +2894,328 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="D1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="K2" t="s">
+        <v>259</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="K3" t="s">
+        <v>255</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="K4" t="s">
+        <v>259</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="K5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B11" t="s">
+        <v>236</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="C12" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="C13" t="s">
+        <v>238</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="C14" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="C15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="D16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="C17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="D18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ny constraints med isCombinedGoalRowAllowed
</commit_message>
<xml_diff>
--- a/concepts/Goal Reduction.xlsx
+++ b/concepts/Goal Reduction.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14895" windowHeight="7875" activeTab="3"/>
@@ -12,12 +12,12 @@
     <sheet name="Statements Empirical" sheetId="3" r:id="rId3"/>
     <sheet name="Combined Goals Reduction" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="258">
   <si>
     <t xml:space="preserve">[[e, inside, l], [l, ontop, g], [g, inside, l], [l, leftof, e], [e, inside, l]], </t>
   </si>
@@ -743,12 +743,6 @@
   </si>
   <si>
     <t>add obj1 to taboolist2</t>
-  </si>
-  <si>
-    <t>if last statement</t>
-  </si>
-  <si>
-    <t>add obj2 to taboolist1</t>
   </si>
   <si>
     <t>Check 1</t>
@@ -802,8 +796,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,16 +831,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -925,6 +924,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -959,6 +959,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1134,21 +1135,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>108</v>
       </c>
@@ -1156,18 +1157,18 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="D5" s="2" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="2:5">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>110</v>
       </c>
@@ -1178,7 +1179,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>111</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>112</v>
       </c>
@@ -1204,7 +1205,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>114</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>116</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>119</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>117</v>
       </c>
@@ -1275,14 +1276,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.42578125" bestFit="1" customWidth="1"/>
@@ -1292,7 +1293,7 @@
     <col min="8" max="8" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1482,7 +1483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1580,7 +1581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1620,7 +1621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1644,7 +1645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1660,7 +1661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1668,7 +1669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1676,7 +1677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1708,7 +1709,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -1724,7 +1725,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -1732,7 +1733,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -1740,7 +1741,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -1756,7 +1757,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>68</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -1796,7 +1797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -1836,292 +1837,292 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2133,21 +2134,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="60" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -2169,7 +2170,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -2224,7 +2225,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -2246,7 +2247,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -2257,7 +2258,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -2268,7 +2269,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>132</v>
       </c>
@@ -2290,7 +2291,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>133</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>135</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -2334,7 +2335,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -2353,7 +2354,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>139</v>
       </c>
@@ -2361,7 +2362,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -2369,7 +2370,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -2393,7 +2394,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>145</v>
       </c>
@@ -2409,7 +2410,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>146</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>148</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -2441,7 +2442,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>150</v>
       </c>
@@ -2449,7 +2450,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>151</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -2473,7 +2474,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>154</v>
       </c>
@@ -2481,7 +2482,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>156</v>
       </c>
@@ -2497,7 +2498,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>157</v>
       </c>
@@ -2505,7 +2506,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>158</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>159</v>
       </c>
@@ -2521,7 +2522,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>160</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -2537,7 +2538,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>162</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>163</v>
       </c>
@@ -2553,7 +2554,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -2561,7 +2562,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>165</v>
       </c>
@@ -2569,7 +2570,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>166</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>167</v>
       </c>
@@ -2585,7 +2586,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>168</v>
       </c>
@@ -2593,7 +2594,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>169</v>
       </c>
@@ -2601,292 +2602,292 @@
         <v>221</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>227</v>
       </c>
@@ -2897,14 +2898,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
@@ -2916,24 +2917,24 @@
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="M1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>230</v>
       </c>
@@ -2943,29 +2944,29 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>246</v>
+      <c r="F2" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>256</v>
+      <c r="J2" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="K2" t="s">
-        <v>259</v>
-      </c>
-      <c r="L2" s="3">
+        <v>257</v>
+      </c>
+      <c r="L2" s="2">
         <v>1</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>230</v>
       </c>
@@ -2975,29 +2976,29 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>256</v>
+      <c r="J3" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="K3" t="s">
-        <v>255</v>
-      </c>
-      <c r="L3" s="3">
+        <v>253</v>
+      </c>
+      <c r="L3" s="2">
         <v>1</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>233</v>
       </c>
@@ -3007,29 +3008,29 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>246</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="K4" t="s">
         <v>257</v>
       </c>
-      <c r="K4" t="s">
-        <v>259</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>233</v>
       </c>
@@ -3039,29 +3040,29 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>247</v>
+      <c r="F5" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>257</v>
+      <c r="J5" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="K5" t="s">
-        <v>255</v>
-      </c>
-      <c r="L5" s="3">
+        <v>253</v>
+      </c>
+      <c r="L5" s="2">
         <v>1</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>234</v>
       </c>
@@ -3071,19 +3072,19 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>246</v>
+      <c r="F6" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>234</v>
       </c>
@@ -3093,19 +3094,19 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>247</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>235</v>
       </c>
@@ -3115,19 +3116,19 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>246</v>
+      <c r="F8" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>235</v>
       </c>
@@ -3137,81 +3138,71 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>247</v>
+      <c r="F9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B11" t="s">
         <v>236</v>
       </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>237</v>
       </c>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>238</v>
       </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>239</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="C17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="D18" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>251</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D21" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="C21" t="s">
-        <v>253</v>
-      </c>
-      <c r="D21" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>